<commit_message>
Updates to code and raw and working data
Inc. finalised quote type counts for a-corpus and corresponding updates to code
</commit_message>
<xml_diff>
--- a/outputs/a/quote_types/list_q_a.xlsx
+++ b/outputs/a/quote_types/list_q_a.xlsx
@@ -11,22 +11,24 @@
     <sheet name="A02 vie saint barbre" sheetId="2" r:id="rId2"/>
     <sheet name="A03 vie saint basille" sheetId="3" r:id="rId3"/>
     <sheet name="A04 vie saint christofle" sheetId="4" r:id="rId4"/>
-    <sheet name="A06 saint jean evangeliste" sheetId="5" r:id="rId5"/>
-    <sheet name="A07 vie saint jean paulus" sheetId="6" r:id="rId6"/>
-    <sheet name="A08 vie glorieux confesseur" sheetId="7" r:id="rId7"/>
-    <sheet name="A09 vie saint leu" sheetId="8" r:id="rId8"/>
-    <sheet name="A11 vie saint sebastien" sheetId="9" r:id="rId9"/>
-    <sheet name="A12 miracle saint servais" sheetId="10" r:id="rId10"/>
-    <sheet name="A13 vie seint thibault" sheetId="11" r:id="rId11"/>
-    <sheet name="A16 guillaume angleterre" sheetId="12" r:id="rId12"/>
-    <sheet name="A17 robert deable" sheetId="13" r:id="rId13"/>
-    <sheet name="A18 richart sans peour" sheetId="14" r:id="rId14"/>
-    <sheet name="A19 elegy troyes" sheetId="15" r:id="rId15"/>
-    <sheet name="A20 vieillards tués" sheetId="16" r:id="rId16"/>
-    <sheet name="A21 mauvais riche homme" sheetId="17" r:id="rId17"/>
-    <sheet name="A22 jeu des dez" sheetId="18" r:id="rId18"/>
-    <sheet name="A23 roy avoit amie" sheetId="19" r:id="rId19"/>
-    <sheet name="A25 quatre sereurs" sheetId="20" r:id="rId20"/>
+    <sheet name="A05 vie sainte dieudonnee" sheetId="5" r:id="rId5"/>
+    <sheet name="A06 saint jean evangeliste" sheetId="6" r:id="rId6"/>
+    <sheet name="A07 vie saint jean paulus" sheetId="7" r:id="rId7"/>
+    <sheet name="A08 vie glorieux confesseur" sheetId="8" r:id="rId8"/>
+    <sheet name="A09 vie saint leu" sheetId="9" r:id="rId9"/>
+    <sheet name="A10 poines enfer" sheetId="10" r:id="rId10"/>
+    <sheet name="A11 vie saint sebastien" sheetId="11" r:id="rId11"/>
+    <sheet name="A12 miracle saint servais" sheetId="12" r:id="rId12"/>
+    <sheet name="A13 vie seint thibault" sheetId="13" r:id="rId13"/>
+    <sheet name="A16 guillaume angleterre" sheetId="14" r:id="rId14"/>
+    <sheet name="A17 robert deable" sheetId="15" r:id="rId15"/>
+    <sheet name="A18 richart sans peour" sheetId="16" r:id="rId16"/>
+    <sheet name="A19 elegy troyes" sheetId="17" r:id="rId17"/>
+    <sheet name="A20 vieillards tués" sheetId="18" r:id="rId18"/>
+    <sheet name="A21 mauvais riche homme" sheetId="19" r:id="rId19"/>
+    <sheet name="A22 jeu des dez" sheetId="20" r:id="rId20"/>
+    <sheet name="A23 roy avoit amie" sheetId="21" r:id="rId21"/>
+    <sheet name="A25 quatre sereurs" sheetId="22" r:id="rId22"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -665,7 +667,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -695,241 +697,121 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Le bourgois a son filz sy a dit sans reprendre:</t>
+          <t>Saint Michel li a dit sans nul delaiement:</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>“Mon enfant, je l'otroy; Dieu, qui se lessa pendre</t>
+          <t>“Sire, cil que vees qui en tenebres sunt,</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>En l'arbre de la croix, te doint si bien aprendre.”</t>
+          <t>Ce sunt li pecheor qui dame Diex meffont.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Qu'il lui face mercy et a tous trespassés.</t>
+          <t>De la paor qu'il ot reclama Damedé:</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>“Ma seur, ce dit le clerc, aveuc moy demourez.”</t>
+          <t>“Merci biaus sire, peres bons roys de maïsté.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>“Par foy,” dit elle, frere, “puis que vous le voulez.</t>
+          <t>Merci biaus sire peres, bons roys de majesté.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Et elle respondi moult delente et marye:</t>
+          <t>Ains que ele ait torné a il dit a sa gent:</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>“En ung puis l'ay jetté, de quoy c'est grant folie.”</t>
+          <t>“Or tost aportés autres tost et isnellement.”</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Quant le clerc l'entendi, si fut moult a malaise.</t>
+          <t>Oiés com grant dolor et grant destrusion:</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>238</v>
+        <v>181</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Qui la mit a raison moult debonairement:</t>
+          <t>Et tuit crient ensamble coume gent tormentee:</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>“Dieu vous gard, christïenne, se lui dist le juïf,</t>
+          <t>“Hai las, chaitive! Ou est la mort alee?</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>J'ay grant pitié de vous par la loy dont je vif.</t>
+          <t>Ici est la mort alee que doit que ne repeire.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>251</v>
+        <v>188</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Celle tout en plourant au juif si respondy:</t>
+          <t>Saint Michiel fu lés li. Saint Pol li demanda:</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>“Et je vous serviray, sire, vostre mercy.”</t>
+          <t>“Qui est cele chaitive qui ce deservi a?”</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>“Or venés aveuc moy,” dit il, “je vous en pry.”</t>
+          <t>Saint Michel li respont: “Ce vous dirai je ja:</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>257</v>
+        <v>458</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>“Tres douche christïenne.” “Par amour,” se dit elle.</t>
+          <t>Li ange le regarde si li a demandé:</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>“Donnez a mon enfant, s'il vous plaist, la mamelle.”</t>
+          <t>“Por quoi pleures, saint Pol? Donc vient ceste tristors?</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Celle si respondi moult debonnairement:</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>259</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Celle si respondi moult debonnairement:</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>“Si feray je, ma dame, sans faire arestement.”</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Lors prist entre ses bras l'enfant moult bonement.</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>297</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Celle si respondy moult debonairement:</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>“Si feray ge, ma dame, du ceur entierement,</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Dieu veille que ce soit tout pour mon sauvement.”</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>311</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Et le juif si respont a basse vois serye:</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>“Ma seur, ce dit le juif, envers moy entendez.</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Dedens nostre jardin, que bien vous le savez,</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>370</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Qui la myt a raison moult debonnairement:</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>“Fame, dit le saint angre, par moy te mande Dieu</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Que tu te reconfortes, et tu en vauldras mieulx.</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12">
-        <v>423</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Jhesuscrist de bon ceur douchement reclama.</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>“Glorieuse vierge, pucelle, fleur de virginité,”</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Se dist la pecheresse, “en qui par amytié</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13">
-        <v>495</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>A tous en general hautement prinst a dire:</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>“Ce corps eust non Servés, d'Alemaigne fut nés,</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>En or et en argent soit richement poses.”</t>
+          <t>Des granz paines d'enfer as veü des gregnors.</t>
         </is>
       </c>
     </row>
@@ -939,6 +821,141 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>line_n</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>prev_line</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>line</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>next_line</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>38</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>On li dist une foiz, quant venoit de chacier:</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>“Sire, vous ne savez, il a un chevalier</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Prez de ci qui a terre molt grant a justicier,</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>66</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Lors saint Sebastien respondi sans demour:</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>“Trop est foul qui aore chose qui n'a valour,</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Om ne doyt aourer que le doulx creatour</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>79</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Quant le tirant l'ouÿ, si li dist par faintise:</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>“Sebastien, amis, je t'aime molt et prise:</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Se te feray haut homme, se fes a mon devise.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>125</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Le bon saint respondi, qui out pensee fine:</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>“Tant plus tormenteras ma char que n'as pas chere,</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Et plus recevra m'ame de perfaite lumiere;</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>225</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Mez je le vous direi, s'entendre le voulez:</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>“Saint Sebastïen, fin et vray, de cuer piteus,</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Je te suppli ou non de Jhesu le vray Diex:</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -970,181 +987,181 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A ceaus qui toi voloient establir de lor mains:</t>
+          <t>Le bourgois a son filz sy a dit sans reprendre:</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>“Ovrez non pas viande, li quels soit trepassable,</t>
+          <t>“Mon enfant, je l'otroy; Dieu, qui se lessa pendre</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Mas cele qui sera toz jors mais pordurable,</t>
+          <t>En l'arbre de la croix, te doint si bien aprendre.”</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>37</v>
+        <v>201</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>As seinz praacheors, bien est chose provee,</t>
+          <t>Et elle respondi moult delente et marye:</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>“De maus m'anvironez, apuiés moi de flor.</t>
+          <t>“En ung puis l'ay jetté, de quoy c'est grant folie.”</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Demandez vos por quoir Quar je languis d'amor.”</t>
+          <t>Quant le clerc l'entendi, si fut moult a malaise.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>271</v>
+        <v>238</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Il reconte, sein Jaque, ce est la veritez:</t>
+          <t>Qui la mit a raison moult debonairement:</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>“Bien aventurez est li honz qui est tentez,</t>
+          <t>“Dieu vous gard, christïenne, se lui dist le juïf,</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Quar, quant il sera bien finement esprovez,</t>
+          <t>J'ay grant pitié de vous par la loy dont je vif.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>329</v>
+        <v>251</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Qui tel chose li distrent com ja dire m'orrez:</t>
+          <t>Celle tout en plourant au juif si respondy:</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>“Graces, beneïcon de Dé omnipotent</t>
+          <t>“Et je vous serviray, sire, vostre mercy.”</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Aies tu, quar tu siers si entenduement;</t>
+          <t>“Or venés aveuc moy,” dit il, “je vous en pry.”</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>341</v>
+        <v>257</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tot en ceste meniere a Odon respondet:</t>
+          <t>“Tres douche christïenne.” “Par amour,” se dit elle.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>“Je redote d'aler contre la volenté</t>
+          <t>“Donnez a mon enfant, s'il vous plaist, la mamelle.”</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>De Dé par cui guinier tu as l'enfermeté;</t>
+          <t>Celle si respondi moult debonnairement:</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>693</v>
+        <v>259</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lo saume do sautier ouquel un tel voirs a:</t>
+          <t>Celle si respondi moult debonnairement:</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>“Jhesu Crist me governe et renz ne me faudra</t>
+          <t>“Si feray je, ma dame, sans faire arestement.”</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Ou lue de cel pasquer ou il m'aloiera.”</t>
+          <t>Lors prist entre ses bras l'enfant moult bonement.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>745</v>
+        <v>297</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>En abit de prevoire, qui tel chose li dit:</t>
+          <t>Celle si respondy moult debonairement:</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>“Odes, resveile toi; or sus, n'endormir mie;</t>
+          <t>“Si feray ge, ma dame, du ceur entierement,</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Pense de fessorer; par tens auras aïe;</t>
+          <t>Dieu veille que ce soit tout pour mon sauvement.”</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>771</v>
+        <v>423</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Par la volenté Dé qui iqui li tramist:</t>
+          <t>Jhesuscrist de bon ceur douchement reclama.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>“Garderres de seint cors, en pensee es grant.</t>
+          <t>“Glorieuse vierge, pucelle, fleur de virginité,”</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Bien ses que tu dois faire. Que vas tu atendant?</t>
+          <t>Se dist la pecheresse, “en qui par amytié</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>889</v>
+        <v>495</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Et ce que vos m'orrois ci dire comencet:</t>
+          <t>A tous en general hautement prinst a dire:</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>“S'i te plait qu'a toi sierve, pere, et en baillie</t>
+          <t>“Ce corps eust non Servés, d'Alemaigne fut nés,</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Ton glorious cors aie, vois moi aparoilie,</t>
+          <t>En or et en argent soit richement poses.”</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1170,222 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>line_n</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>prev_line</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>line</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>next_line</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>17</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>A ceaus qui toi voloient establir de lor mains:</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>“Ovrez non pas viande, li quels soit trepassable,</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Mas cele qui sera toz jors mais pordurable,</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>37</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>As seinz praacheors, bien est chose provee,</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>“De maus m'anvironez, apuiés moi de flor.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Demandez vos por quoir Quar je languis d'amor.”</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>271</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Il reconte, sein Jaque, ce est la veritez:</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>“Bien aventurez est li honz qui est tentez,</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Quar, quant il sera bien finement esprovez,</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>329</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Qui tel chose li distrent com ja dire m'orrez:</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>“Graces, beneïcon de Dé omnipotent</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Aies tu, quar tu siers si entenduement;</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>341</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tot en ceste meniere a Odon respondet:</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>“Je redote d'aler contre la volenté</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>De Dé par cui guinier tu as l'enfermeté;</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>693</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Lo saume do sautier ouquel un tel voirs a:</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>“Jhesu Crist me governe et renz ne me faudra</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Ou lue de cel pasquer ou il m'aloiera.”</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>745</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>En abit de prevoire, qui tel chose li dit:</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>“Odes, resveile toi; or sus, n'endormir mie;</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Pense de fessorer; par tens auras aïe;</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>771</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Par la volenté Dé qui iqui li tramist:</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>“Garderres de seint cors, en pensee es grant.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Bien ses que tu dois faire. Que vas tu atendant?</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>889</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Et ce que vos m'orrois ci dire comencet:</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>“S'i te plait qu'a toi sierve, pere, et en baillie</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Ton glorious cors aie, vois moi aparoilie,</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -1189,337 +1421,337 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Le prestre qui fu sage tantost li respondi</t>
+          <t>Le prestre, qui fu sage, tantost li respondi:</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>“Mon seingneur je me dout par la Vierge Marie</t>
+          <t>“Mon seingneur, je me dout, par la Vierge Marie,</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Que celle vois ne veingne par art de diablie</t>
+          <t>Que celle vois ne veingne par art de diablie;</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Hautement a parlé et dist Guillaume roys</t>
+          <t>Et li dist en quel guisse la vois fu revenue.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>“Voir il te mescherra briément ce ne mécrois</t>
+          <t>“Trop forment me menace, se je ne me remue.”</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Dieu veult qu'en essil voisses fous es quant tu n'i vas</t>
+          <t>Quant son comfessour ot la parole entendue,</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>138</v>
+        <v>182</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Et li dist en quel guisse la vois fu revenue</t>
+          <t>Quel part vouloit aler; et le roy li respont:</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>“Trop forment me menace se je ne me remue”</t>
+          <t>“Dame, a matines vois; car par temps sonneront.”</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Quant son comfessour ot la parole entendue</t>
+          <t>“Hé! roy, dist la roïne, vos amours fausses sont;</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>177</v>
+        <v>281</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bas dist en soupirant douce suer je m'en vois</t>
+          <t>Quant elle s'esveilla, a haute vois s'escrie:</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>“Douce ami loiale jamés ne vous verré</t>
+          <t>“Hé, tres dous Roi de gloire! je m'esrage de fain;</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Ne le fruit que j'avoie dedens vous engendré”</t>
+          <t>Mourir me couvandra, se briement n'ai du pain.”</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>182</v>
+        <v>314</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Quel part vouloit aler et le roy li respont</t>
+          <t>Quant le roy vint pres d'eus, moult doucement leur prie:</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>“Dame a matines vois car par temps sonneront”</t>
+          <t>“Seingneurs, pour l'amour du tres dous Jhesucrist,</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>“Hé; roy dist la roine vos amours fausses sont</t>
+          <t>Donnés moi de vos pain, s'il vous plest, un petit.”</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>281</v>
+        <v>317</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Quant elle s'esveilla a haute vois s'escrie</t>
+          <t>Lors un mauvés glouton s'escria par despit:</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>“Hé; tres dous roi de gloire je m'esrage de fain</t>
+          <t>“Biau seingneurs, regardez, pour Dieu, com fait truant:</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Mourir me couvandra se briement n'ai du pain”</t>
+          <t>Trop est fort et delivre, et va son pain querant!</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Quant le roy vint prés d'eus moult doucement leur prie</t>
+          <t>Un autre respondi qui estoit plus sachant:</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>“Seingneurs pour l'amour du tres dous Jhesucrist</t>
+          <t>“Sire, que savez vous s'il set point de mestier?</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Donnés moi de vos pain s'il vous plest un petit”</t>
+          <t>Espoir qui ne fist onques fors que lui pourchacier;</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Lors un mauvés glouton s'escria par despit</t>
+          <t>Le bon roy d'Engleterre parla moult doucement:</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>“Biau seingneurs regardez pour Dieu com fait truant</t>
+          <t>“Sire, foy que doi Dieu, je n'ai pain ne argent.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Trop est fort et delivre et va son pain quérant</t>
+          <t>Pour Dieu vous en requier, s'en avés aissement.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Un autre respondi qui estoit plus sachant</t>
+          <t>Lors un mauvés glouton a haute vois c'escrie:</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>“Sire que savez vous s'il set point de mestier</t>
+          <t>“Certes, n'as pas ta lengue pour ton escot laissie.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Espoir qui ne fist onques fors que lui pourchacier</t>
+          <t>Les bribes qu'as mengiés ne comteroie mie.”</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Le bon roy d'Engleterre parla moult doucement</t>
+          <t>Le roy, qui ot grant duel, doucement respondi:</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>“Sire foy que doi Dieu je n'ai pain ne argent</t>
+          <t>“Seingneurs, puis qu'il vous plest, bien weil qu'il soit ainsi;</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Pour Dieu vous en requier s'en avés aissement</t>
+          <t>Mes pour l'amor de Dieu aiez de nous merci,</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>331</v>
+        <v>366</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Lors un mauvés glouton a haute vois c'escrie</t>
+          <t>Et puis si li crierent hautement, non pas bas:</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>“Certes n'as pas ta lengue pour ton escot laissie</t>
+          <t>“La dame enporteron, jamés ne la verras.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Les bribes qu'as mengiés ne comteroie mie”</t>
+          <t>Les batars te lairons. Par les moustiers iras;</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>366</v>
+        <v>456</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Et puis si li crierent hautement non pas bas</t>
+          <t>Il se mist a genous, puis a dist en tel guisse:</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>“La dame enporteron jamés ne la verras</t>
+          <t>“Tres dous Dieus, gardé moy de male couvoitise.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Les batars te lairons par les moustiers iras</t>
+          <t>J'ai aujourd'ui perdu ma fame et mes enfans.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>456</v>
+        <v>532</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Il se mist a genous puis a dist en tel guisse</t>
+          <t>Il dist a la roïne qu'il veoit bien aprisse:</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>“Tres dous Dieus gardé moy de male couvoitise</t>
+          <t>“Ma suer, vous savez bien en quel lieu vous ai prisse.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>J'ai aujourd'ui perdu ma fame et mes enfans</t>
+          <t>Voir, je ne sai dont estes ne de quel parenté;</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>532</v>
+        <v>722</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Il dist a la roine qu'il veoit bien aprisse</t>
+          <t>L'un des enfans li dist, qui estoit le plus sage:</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>“Ma suer vous savez bien en quel lieu vous ai prisse</t>
+          <t>“Sire, de vous servir ai moult tres bon courage.”</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Voir je ne sai dont estes ne de quel parenté</t>
+          <t>Le conte les mena en son mestre menage,</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>722</v>
+        <v>761</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>L'un des enfans li dist qui estoit le plus sage</t>
+          <t>Lors l'apella le roy, moult doucement li dist:</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>“Sire de vous servir ai moult tres bon courage”</t>
+          <t>“Biaus amis, voulez vous cel cor d'ivoire vendre?”</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Le conte les mena en son mestre menage</t>
+          <t>Et il li respondi: “Ouil,” sans plus atendre.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>761</v>
+        <v>770</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Lors l'apella le roy moult doucement li dist</t>
+          <t>Quant le roy l'entendi, si li a respondu:</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>“Biaus amis voulez vous cel cor d'ivoire vendre”</t>
+          <t>“Est donques celui mort a qui ce cornet fu?”</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Et il li respondi “Ouil” sans plus atendre</t>
+          <t>“Ouil, sire,” dist il, “puis qu'il n'est revenu.”</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>770</v>
+        <v>818</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Quant le roy l'entendi si li a respondu</t>
+          <t>La dame vint au roy et li a dit moult bel:</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>“Est donques celui mort a qui ce cornet fu”</t>
+          <t>“Sire, se vous voulés aquiter cest vessel,</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>“Ouil sire dist il puis qu'il n'est revenu”</t>
+          <t>J'aurai de vostre doi seulement cel anel,</t>
         </is>
       </c>
     </row>
@@ -1529,17 +1761,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>S'il qui fu plus hastis s'escria a haut ton</t>
+          <t>Sil qui fu plus hastis s'escria a haut ton:</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>“Sire vostre filz sui de certain le penson</t>
+          <t>“Sire, vostre filz sui de certain le penson.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Rescous fui a un leu qui m'avoit engoulé</t>
+          <t>Rescous fui a un leu qui m'avoit engoulé;</t>
         </is>
       </c>
     </row>
@@ -1549,17 +1781,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>De cuer leur pardonna et puis leur dist ainsi</t>
+          <t>De cuer leur pardonna, et puis leur dist ainsi:</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>“Biaus enfans je vous lo qu'aillons sans nul detri</t>
+          <t>“Biaus enfans, je vous lo qu'aillons sans nul detri</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Parler a votre mere le plus tost que pourron</t>
+          <t>Parler a votre mere le plus tost que pourron;</t>
         </is>
       </c>
     </row>
@@ -1568,7 +1800,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -1604,17 +1836,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Que il se mariast; mais il dist a cler son</t>
+          <t>Que il se mariast; mais il dist a cler son:</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>“Seignour a vostre los. de gré me mariasse</t>
+          <t>“Seignour, a vostre los de gré me mariasse,</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Se partie endroit moi; seusse ne trouvaisse</t>
+          <t>Se partie endroit moi seusse ne trouvaisse;</t>
         </is>
       </c>
     </row>
@@ -1624,17 +1856,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>La ducesse l'oÿ; si dist a voiz serie.</t>
+          <t>La ducesse l'oÿ si dist a voiz serie:</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>“Voir en gré nous faut prendre ce que Diex nous envoie”</t>
+          <t>“Voir en gré nous faut prendre ce que Diex nous envoie.”</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Le duc ala chacier a qui forment anoie</t>
+          <t>Le duc ala chacier a qui forment anoie;</t>
         </is>
       </c>
     </row>
@@ -1644,17 +1876,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>La duchesse parla. et dist com fole femme</t>
+          <t>La duchesse parla et dist com fole femme:</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>“Mais tout soit au dëable qui ne quiert que diffame</t>
+          <t>“Mais tout soit au deable qui ne quiert que diffame.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Puis que Diex n'a puissance que nus enfans nous doint</t>
+          <t>Puis que Diex n'a puissance que nus enfans nous doint,</t>
         </is>
       </c>
     </row>
@@ -1664,17 +1896,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>La duchesse disoit quant vint au travaillier</t>
+          <t>La duchesse disoit quant vint au travaillier:</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>“Lasse d'avoir enfant avoie grant mestier</t>
+          <t>“Lasse, d'avoir enfant avoie grant mestier,</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Voir grant desir avoie de ma mort auancier”</t>
+          <t>Voir grant desir avoie de ma mort avancier.”</t>
         </is>
       </c>
     </row>
@@ -1684,17 +1916,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Lors Robert le dëable; respondi par folour</t>
+          <t>Lors Robert le deable respondi par folour:</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>“Pere de moi blamer vous povez trop bien taire</t>
+          <t>“Pere, de moi blamer vous povez trop bien taire.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Vouz perdez vostre paine n'ai talent de bien faire</t>
+          <t>Vouz perdez vostre paine, n'ai talent de bien faire.</t>
         </is>
       </c>
     </row>
@@ -1704,17 +1936,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Les chevaliers disoient touz bas a leur mesnie</t>
+          <t>Les chevaliers disoient touz bas a leur mesnie:</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>“Quant ce dyable vient nous n'assamblerons mie</t>
+          <t>“Quant ce dyable vient, nous n'assamblerons mie;</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Prier estuet que Diex li envoit courte vie.</t>
+          <t>Prier estuet que Diex li envoit courte vie,</t>
         </is>
       </c>
     </row>
@@ -1724,17 +1956,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Que Robert leur faisoit l'un d'eulz dist a cler son.</t>
+          <t>Que Robert leur faisoit. L'un d'eulz dist a cler son:</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>“Franc duc Robert vo filz prent a force nos femmes</t>
+          <t>“Franc duc, Robert vo filz prent a force nos femmes,</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Nos filles et nos nieces trop est grant li difames</t>
+          <t>Nos filles et nos nieces; trop est grant li difames,</t>
         </is>
       </c>
     </row>
@@ -1744,17 +1976,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Fist traire les .ii. yex et puis si leur a dist</t>
+          <t>Fist traire les deus yex et puis si leur a dist:</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>“Vous endormirez miex demain en vostre lit</t>
+          <t>“Vous endormirez miex demain en vostre lit;</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Mais dites a mon pere que c'est en son despit”</t>
+          <t>Mais dites a mon pere que c'est en son despit.”</t>
         </is>
       </c>
     </row>
@@ -1764,17 +1996,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>L'un des larrons parla; et dist sanz alentir</t>
+          <t>L'un des larrons parla et dist sanz alentir:</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>“Je croi que Renart veut hermite devenir</t>
+          <t>“Je croi que Renart veut hermite devenir.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Robert qui estoit yer. le pire de nous touz</t>
+          <t>Robert qui estoit yer le pire de nous touz</t>
         </is>
       </c>
     </row>
@@ -1784,17 +2016,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Robert s'agenoulla et leur dist doucement</t>
+          <t>Robert s'agenoulla et leur dist doucement:</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>“Je vous requier merci pour Dieu omnipotent</t>
+          <t>“Je vous requier merci, pour Dieu omnipotent,</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Car je vous ai a tort par plusieurs foiz grevez”</t>
+          <t>Car je vous ai a tort par plusieurs foiz grevez.”</t>
         </is>
       </c>
     </row>
@@ -1804,17 +2036,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Contreface le fol s'il veult que sauvé soit</t>
+          <t>Contreface le fol, s'il veult que sauvé soit.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>“Et que il ne menguce. ne pain ne autre biens</t>
+          <t>“Et que il ne menguce. ne pain ne autre biens,</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>S'il ne le puet tolir ou esrachier aus chiens.</t>
+          <t>S'il ne le puet tolir ou esrachier aus chiens,</t>
         </is>
       </c>
     </row>
@@ -1824,7 +2056,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>L'emperere le vit si dist de cuer ouvert</t>
+          <t>L'emperere le vit, si dist de cuer ouvert:</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1834,7 +2066,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Lors l'en aporta .i. un varlet plus apert</t>
+          <t>Lors l'en aporta un un varlet plus apert.</t>
         </is>
       </c>
     </row>
@@ -1844,17 +2076,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Mais non pour tant il dist a sa chevalerie</t>
+          <t>Mais non pour tant il dist a sa chevalerie:</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>“Je vous pri biax seignors que nous nous ensaions</t>
+          <t>“Je vous pri, biax seignors, que nous nous ensaions,</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Contre ces Sarrazins nostre droit deffendons”</t>
+          <t>Contre ces sarrazins nostre droit deffendons.”</t>
         </is>
       </c>
     </row>
@@ -1864,17 +2096,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Et comment en sa cuisse mist le fer de sa lance</t>
+          <t>Et comment en sa cuisse mist le fer de sa lance:</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>“Je me repent forment que je l'ai fait grevance</t>
+          <t>“Je me repent forment que je l'ai fait grevance,</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>La mere Dieu la veille deffendre de meschance</t>
+          <t>La mere Dieu la veille deffendre de meschance.</t>
         </is>
       </c>
     </row>
@@ -1884,17 +2116,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Il vint a l'emperere et li dist hautement</t>
+          <t>Il vint a l'emperere et li dist hautement:</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>“Sire je sui celui qui s'en vint a l'asaut</t>
+          <t>“Sire, je sui celui qui s'en vint a l'asaut</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Par .iii. foiz sus Paiens moult y souffri de chaut.”</t>
+          <t>Par trois foiz sus paiens; moult y souffri de chaut.”</t>
         </is>
       </c>
     </row>
@@ -1904,17 +2136,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Tantost qu'il vit Robert si li a dit ces mos.</t>
+          <t>Tantost qu'il vit Robert, si li a dit ces mos:</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>“Amis entendez moi moult bien vous connoissons</t>
+          <t>“Amis, entendez moi, moult bien vous connoissons.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Voir Robert le dëable soloit estre vos nons</t>
+          <t>Voir Robert le deable soloit estre vos nons;</t>
         </is>
       </c>
     </row>
@@ -1924,17 +2156,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Il s'aprocha de li. et fierement li dist</t>
+          <t>Il s'aprocha de li et fierement li dist:</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>“Pas ne m'eschaperez a cel coup que je puisse</t>
+          <t>“Pas ne m'eschaperez a cel coup que je puisse!</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Ne boutas tu le fer; d'une lance en ta cuisse</t>
+          <t>Ne boutas tu le fer d'une lance en ta cuisse?</t>
         </is>
       </c>
     </row>
@@ -1943,9 +2175,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2015,99 +2247,119 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>497</v>
+        <v>409</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Reconforter alla le franc duc de renom:</t>
+          <t>Le corps qui gisoit la s'escria hautement:</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>“Sire, n'ayés frayour, doubte ne souspecon!</t>
+          <t>“Et comment, duc Richart, ouvrés vous tellement?</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Les ennemis d'enfer ont povoir, se savon,</t>
+          <t>On parle en tous paÿs de vostre hardement,</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>554</v>
+        <v>497</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Le noir chevallier dist a moult haulte raison:</t>
+          <t>Reconforter alla le franc duc de renom:</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>“J'ay a nom Brundemor, point ne vous celleron.</t>
+          <t>“Sire, n'ayés frayour, doubte ne souspecon!</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Quant nous serons en guerre se ne vous doubtés mie</t>
+          <t>Les ennemis d'enfer ont povoir, se savon,</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Quant Brundemort vot ce hautement leur estrie:</t>
+          <t>Le noir chevallier dist a moult haulte raison:</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>“Si n'y a nul de vous qui soit garny d'amye,</t>
+          <t>“J'ay a nom Brundemor, point ne vous celleron.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Qui aime par amours, viengne a moy si guerrie.”</t>
+          <t>Quant nous serons en guerre se ne vous doubtés mie</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>637</v>
+        <v>569</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ung varlet parmy l'ost s'en va venir criant:</t>
+          <t>Quant Brundemort vot ce hautement leur estrie:</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>“Brundemor, ou es tu? Que vas tu tant tardant</t>
+          <t>“Si n'y a nul de vous qui soit garny d'amye,</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Que tost ne nous amaines ton chevallier errant</t>
+          <t>Qui aime par amours, viengne a moy si guerrie.”</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8">
+        <v>637</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Ung varlet parmy l'ost s'en va venir criant:</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>“Brundemor, ou es tu? Que vas tu tant tardant</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Que tost ne nous amaines ton chevallier errant</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
         <v>777</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>Et quant Richart l'entant a haulte voix s'escrie:</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>“Rens donc a Brundemor tost sa seneschaussie</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Que faulcement luy as par ta force ravie.”</t>
         </is>
@@ -2118,7 +2370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -2213,7 +2465,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2288,7 +2540,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -2395,116 +2647,6 @@
       <c r="D5" t="inlineStr">
         <is>
           <t>Las, pourray je jamais de ce tourmant yssir?</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>line_n</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>prev_line</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>line</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>next_line</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>line_n</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>prev_line</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>line</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>next_line</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
-        <v>49</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Qe homage e service du chevaler enquist.</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>“Avay! sir Belial, tu queres grant utrage,”</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Dist le chevaler, “qe fust de fere curage;</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>160</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Doucement respount ly curtoise chevaler:</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>“E jeo le vus pardonne fraunchement de qoer,</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Vus me avez costé mut chier huy cest jour:</t>
         </is>
       </c>
     </row>
@@ -2690,6 +2832,116 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>line_n</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>prev_line</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>line</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>next_line</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>line_n</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>prev_line</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>line</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>next_line</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>49</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Qe homage e service du chevaler enquist.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>“Avay! sir Belial, tu queres grant utrage,”</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Dist le chevaler, “qe fust de fere curage;</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>160</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Doucement respount ly curtoise chevaler:</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>“E jeo le vus pardonne fraunchement de qoer,</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Vus me avez costé mut chier huy cest jour:</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3215,6 +3467,221 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>line_n</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>prev_line</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>line</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>next_line</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>121</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Quart li curés l'oï, se li respondi lors:</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>“Vous yestes bielle et boine, si plest a Dieu, m'amie.”</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>La damme li dist: “Sire, ne me respondés mie</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>245</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Que c'avoit fait Jehan, qui sa mere pierdi.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>“Sa mere avoit des gens mout boine renommee,</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Puis s'enfuï par nuit, ses fieus m'a encantee.”</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>297</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Qu'elle le hierbegast ou non de Jhesucrist,</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>“En si faitte maniere que Dieus vous laist joïr</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>De le cose dou monde dont plus avés desir.”</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>361</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Doucement l'efforca, en souspirant li dist:</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>“Megniés, ma douce soer, car je vous ay couvent</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Que vous n'arés defaute de riens qui soit ceens,</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>434</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Lors la mere a sa fille respondi en plorant:</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>“L'evesque venra chi, n'ira gaires targant;</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Ma suer, bien vous en croi quant me proumetés tant,</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>564</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Puis oï une vois qui li dist en oiant:</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>“Bielle suer, fai grant joie, ne te va esmaiant.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Pour les honneurs mondaines dont tu yes traite ariere</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>648</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Elle oÿ une vois qui doucement li dist:</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>“Dieudenee, ma fille, mout as souffiert labit;</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Nostre Sires vous mande que demain a midi</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>655</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Tout au mieus qu'elle pot, dist a sa cambouriere:</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>“Va tos quere la damme, di li en tel maniere,</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Que s'oncques a nul jour eut Dieudonnee ciere,</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>674</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Quant elle peut parler, haut dist ses poins tordant:</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>“Que m'est il avenut, quetive meskeant?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Ne pooie connoistre en vie mon enfant,</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3348,7 +3815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -3543,7 +4010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3618,7 +4085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -3711,139 +4178,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>line_n</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>prev_line</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>line</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>next_line</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
-        <v>38</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>On li dist une foiz, quant venoit de chacier:</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>“Sire, vous ne savez, il a un chevalier</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Prez de ci qui a terre molt grant a justicier,</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>66</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Lors saint Sebastien respondi sans demour:</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>“Trop est foul qui aore chose qui n'a valour,</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Om ne doyt aourer que le doulx creatour</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>79</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Quant le tirant l'ouÿ, si li dist par faintise:</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>“Sebastien, amis, je t'aime molt et prise:</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Se te feray haut homme, se fes a mon devise.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>125</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Le bon saint respondi, qui out pensee fine:</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>“Tant plus tormenteras ma char que n'as pas chere,</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Et plus recevra m'ame de perfaite lumiere;</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>225</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Mez je le vous direi, s'entendre le voulez:</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>“Saint Sebastïen, fin et vray, de cuer piteus,</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Je te suppli ou non de Jhesu le vray Diex:</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated outputs and code
</commit_message>
<xml_diff>
--- a/outputs/a/quote_types/list_q_a.xlsx
+++ b/outputs/a/quote_types/list_q_a.xlsx
@@ -12,23 +12,24 @@
     <sheet name="A03 vie saint basille" sheetId="3" r:id="rId3"/>
     <sheet name="A04 vie saint christofle" sheetId="4" r:id="rId4"/>
     <sheet name="A05 vie sainte dieudonnee" sheetId="5" r:id="rId5"/>
-    <sheet name="A06 saint jean evangeliste" sheetId="6" r:id="rId6"/>
-    <sheet name="A07 vie saint jean paulus" sheetId="7" r:id="rId7"/>
-    <sheet name="A08 vie glorieux confesseur" sheetId="8" r:id="rId8"/>
-    <sheet name="A09 vie saint leu" sheetId="9" r:id="rId9"/>
-    <sheet name="A10 poines enfer" sheetId="10" r:id="rId10"/>
-    <sheet name="A11 vie saint sebastien" sheetId="11" r:id="rId11"/>
-    <sheet name="A12 miracle saint servais" sheetId="12" r:id="rId12"/>
-    <sheet name="A13 vie seint thibault" sheetId="13" r:id="rId13"/>
-    <sheet name="A16 guillaume angleterre" sheetId="14" r:id="rId14"/>
-    <sheet name="A17 robert deable" sheetId="15" r:id="rId15"/>
-    <sheet name="A18 richart sans peour" sheetId="16" r:id="rId16"/>
-    <sheet name="A19 elegy troyes" sheetId="17" r:id="rId17"/>
-    <sheet name="A20 vieillards tués" sheetId="18" r:id="rId18"/>
-    <sheet name="A21 mauvais riche homme" sheetId="19" r:id="rId19"/>
-    <sheet name="A22 jeu des dez" sheetId="20" r:id="rId20"/>
-    <sheet name="A23 roy avoit amie" sheetId="21" r:id="rId21"/>
-    <sheet name="A25 quatre sereurs" sheetId="22" r:id="rId22"/>
+    <sheet name="A06 vie saint gregoire" sheetId="6" r:id="rId6"/>
+    <sheet name="A07 saint jean evangeliste" sheetId="7" r:id="rId7"/>
+    <sheet name="A08 vie saint jean paulus" sheetId="8" r:id="rId8"/>
+    <sheet name="A09 vie glorieux confesseur" sheetId="9" r:id="rId9"/>
+    <sheet name="A10 vie saint leu" sheetId="10" r:id="rId10"/>
+    <sheet name="A11 poines enfer" sheetId="11" r:id="rId11"/>
+    <sheet name="A12 vie saint sebastien" sheetId="12" r:id="rId12"/>
+    <sheet name="A13 miracle saint servais" sheetId="13" r:id="rId13"/>
+    <sheet name="A14 vie seint thibault" sheetId="14" r:id="rId14"/>
+    <sheet name="A17 guillaume angleterre" sheetId="15" r:id="rId15"/>
+    <sheet name="A18 robert deable" sheetId="16" r:id="rId16"/>
+    <sheet name="A19 richart sans peour" sheetId="17" r:id="rId17"/>
+    <sheet name="A20 elegy troyes" sheetId="18" r:id="rId18"/>
+    <sheet name="A21 vieillards tués" sheetId="19" r:id="rId19"/>
+    <sheet name="A22 mauvais riche homme" sheetId="20" r:id="rId20"/>
+    <sheet name="A23 jeu des dez" sheetId="21" r:id="rId21"/>
+    <sheet name="A24 roy avoit amie" sheetId="22" r:id="rId22"/>
+    <sheet name="A26 quatre sereurs" sheetId="23" r:id="rId23"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -667,6 +668,101 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>line_n</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>prev_line</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>line</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>next_line</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>151</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>L'annel boute en son dois, puis leur dist maintenant:</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>“Seigneurs, comment se porte l'eglise et la gent?”</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Et il ont respondu: “Sire, moult flebement.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>177</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>L'archevesque saint Leu si lui a repondu:</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>“Coulombe, belle suer, chascun si doit mater</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Sa charongne pour Dieu servir et hounourer.”</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>217</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Tout fu prest a cuilir, ce fu grace plainiere.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>“Encore vous requier par sainte trinité</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Que toutes creatures qui seront tourmenté</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -820,7 +916,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -947,221 +1043,6 @@
       <c r="D6" t="inlineStr">
         <is>
           <t>Je te suppli ou non de Jhesu le vray Diex:</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>line_n</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>prev_line</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>line</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>next_line</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
-        <v>25</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Le bourgois a son filz sy a dit sans reprendre:</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>“Mon enfant, je l'otroy; Dieu, qui se lessa pendre</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>En l'arbre de la croix, te doint si bien aprendre.”</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>201</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Et elle respondi moult delente et marye:</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>“En ung puis l'ay jetté, de quoy c'est grant folie.”</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Quant le clerc l'entendi, si fut moult a malaise.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>238</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Qui la mit a raison moult debonairement:</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>“Dieu vous gard, christïenne, se lui dist le juïf,</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>J'ay grant pitié de vous par la loy dont je vif.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>251</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Celle tout en plourant au juif si respondy:</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>“Et je vous serviray, sire, vostre mercy.”</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>“Or venés aveuc moy,” dit il, “je vous en pry.”</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>257</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>“Tres douche christïenne.” “Par amour,” se dit elle.</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>“Donnez a mon enfant, s'il vous plaist, la mamelle.”</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Celle si respondi moult debonnairement:</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>259</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Celle si respondi moult debonnairement:</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>“Si feray je, ma dame, sans faire arestement.”</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Lors prist entre ses bras l'enfant moult bonement.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>297</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Celle si respondy moult debonairement:</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>“Si feray ge, ma dame, du ceur entierement,</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Dieu veille que ce soit tout pour mon sauvement.”</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>423</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Jhesuscrist de bon ceur douchement reclama.</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>“Glorieuse vierge, pucelle, fleur de virginité,”</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Se dist la pecheresse, “en qui par amytié</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>495</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>A tous en general hautement prinst a dire:</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>“Ce corps eust non Servés, d'Alemaigne fut nés,</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>En or et en argent soit richement poses.”</t>
         </is>
       </c>
     </row>
@@ -1202,181 +1083,181 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A ceaus qui toi voloient establir de lor mains:</t>
+          <t>Le bourgois a son filz sy a dit sans reprendre:</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>“Ovrez non pas viande, li quels soit trepassable,</t>
+          <t>“Mon enfant, je l'otroy; Dieu, qui se lessa pendre</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Mas cele qui sera toz jors mais pordurable,</t>
+          <t>En l'arbre de la croix, te doint si bien aprendre.”</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>37</v>
+        <v>201</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>As seinz praacheors, bien est chose provee,</t>
+          <t>Et elle respondi moult delente et marye:</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>“De maus m'anvironez, apuiés moi de flor.</t>
+          <t>“En ung puis l'ay jetté, de quoy c'est grant folie.”</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Demandez vos por quoir Quar je languis d'amor.”</t>
+          <t>Quant le clerc l'entendi, si fut moult a malaise.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>271</v>
+        <v>238</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Il reconte, sein Jaque, ce est la veritez:</t>
+          <t>Qui la mit a raison moult debonairement:</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>“Bien aventurez est li honz qui est tentez,</t>
+          <t>“Dieu vous gard, christïenne, se lui dist le juïf,</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Quar, quant il sera bien finement esprovez,</t>
+          <t>J'ay grant pitié de vous par la loy dont je vif.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>329</v>
+        <v>251</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Qui tel chose li distrent com ja dire m'orrez:</t>
+          <t>Celle tout en plourant au juif si respondy:</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>“Graces, beneïcon de Dé omnipotent</t>
+          <t>“Et je vous serviray, sire, vostre mercy.”</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Aies tu, quar tu siers si entenduement;</t>
+          <t>“Or venés aveuc moy,” dit il, “je vous en pry.”</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>341</v>
+        <v>257</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tot en ceste meniere a Odon respondet:</t>
+          <t>“Tres douche christïenne.” “Par amour,” se dit elle.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>“Je redote d'aler contre la volenté</t>
+          <t>“Donnez a mon enfant, s'il vous plaist, la mamelle.”</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>De Dé par cui guinier tu as l'enfermeté;</t>
+          <t>Celle si respondi moult debonnairement:</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>693</v>
+        <v>259</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lo saume do sautier ouquel un tel voirs a:</t>
+          <t>Celle si respondi moult debonnairement:</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>“Jhesu Crist me governe et renz ne me faudra</t>
+          <t>“Si feray je, ma dame, sans faire arestement.”</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Ou lue de cel pasquer ou il m'aloiera.”</t>
+          <t>Lors prist entre ses bras l'enfant moult bonement.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>745</v>
+        <v>297</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>En abit de prevoire, qui tel chose li dit:</t>
+          <t>Celle si respondy moult debonairement:</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>“Odes, resveile toi; or sus, n'endormir mie;</t>
+          <t>“Si feray ge, ma dame, du ceur entierement,</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Pense de fessorer; par tens auras aïe;</t>
+          <t>Dieu veille que ce soit tout pour mon sauvement.”</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>771</v>
+        <v>423</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Par la volenté Dé qui iqui li tramist:</t>
+          <t>Jhesuscrist de bon ceur douchement reclama.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>“Garderres de seint cors, en pensee es grant.</t>
+          <t>“Glorieuse vierge, pucelle, fleur de virginité,”</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Bien ses que tu dois faire. Que vas tu atendant?</t>
+          <t>Se dist la pecheresse, “en qui par amytié</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>889</v>
+        <v>495</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Et ce que vos m'orrois ci dire comencet:</t>
+          <t>A tous en general hautement prinst a dire:</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>“S'i te plait qu'a toi sierve, pere, et en baillie</t>
+          <t>“Ce corps eust non Servés, d'Alemaigne fut nés,</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Ton glorious cors aie, vois moi aparoilie,</t>
+          <t>En or et en argent soit richement poses.”</t>
         </is>
       </c>
     </row>
@@ -1386,6 +1267,221 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>line_n</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>prev_line</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>line</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>next_line</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>17</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>A ceaus qui toi voloient establir de lor mains:</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>“Ovrez non pas viande, li quels soit trepassable,</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Mas cele qui sera toz jors mais pordurable,</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>37</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>As seinz praacheors, bien est chose provee,</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>“De maus m'anvironez, apuiés moi de flor.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Demandez vos por quoir Quar je languis d'amor.”</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>271</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Il reconte, sein Jaque, ce est la veritez:</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>“Bien aventurez est li honz qui est tentez,</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Quar, quant il sera bien finement esprovez,</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>329</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Qui tel chose li distrent com ja dire m'orrez:</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>“Graces, beneïcon de Dé omnipotent</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Aies tu, quar tu siers si entenduement;</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>341</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tot en ceste meniere a Odon respondet:</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>“Je redote d'aler contre la volenté</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>De Dé par cui guinier tu as l'enfermeté;</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>693</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Lo saume do sautier ouquel un tel voirs a:</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>“Jhesu Crist me governe et renz ne me faudra</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Ou lue de cel pasquer ou il m'aloiera.”</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>745</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>En abit de prevoire, qui tel chose li dit:</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>“Odes, resveile toi; or sus, n'endormir mie;</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Pense de fessorer; par tens auras aïe;</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>771</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Par la volenté Dé qui iqui li tramist:</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>“Garderres de seint cors, en pensee es grant.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Bien ses que tu dois faire. Que vas tu atendant?</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>889</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Et ce que vos m'orrois ci dire comencet:</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>“S'i te plait qu'a toi sierve, pere, et en baillie</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Ton glorious cors aie, vois moi aparoilie,</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -1471,7 +1567,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>“Hé! roy, dist la roïne, vos amours fausses sont;</t>
+          <t>“Hé! roy,” dist la roïne, “vos amours fausses sont;</t>
         </is>
       </c>
     </row>
@@ -1800,7 +1896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -2175,7 +2271,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -2370,7 +2466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -2465,7 +2561,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2532,121 +2628,6 @@
       <c r="D3" t="inlineStr">
         <is>
           <t>De quanque il puet faire fait il le mien coumant,</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>line_n</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>prev_line</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>line</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>next_line</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
-        <v>6</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Le ladre au riche homme fist un courtois reclain:</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>“En l'enneur de Dieu qui est le roy souverain,</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Donne moy, se te plait, un peu de menu pain.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>32</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Ce respont le riche hom qui fu fel et puant:</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>“Suy je doncques tenuz a paistre ce truant,</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ce mesel, contrefait, avulgle, caÿmant,</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>50</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Au ladre les hara sans point de l'atargier.</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>“Va tantost, si me hare mez chiens a ce mesel</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Qui par devant ma porte demaine tel cembel,</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>83</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Souvent se claime las, chetis, maleüreux</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>“Que feray, que diray, que pourray devenir?</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Las, pourray je jamais de ce tourmant yssir?</t>
         </is>
       </c>
     </row>
@@ -2832,6 +2813,121 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>line_n</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>prev_line</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>line</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>next_line</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Le ladre au riche homme fist un courtois reclain:</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>“En l'enneur de Dieu qui est le roy souverain,</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Donne moy, se te plait, un peu de menu pain.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>32</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Ce respont le riche hom qui fu fel et puant:</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>“Suy je doncques tenuz a paistre ce truant,</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ce mesel, contrefait, avulgle, caÿmant,</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>50</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Au ladre les hara sans point de l'atargier.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>“Va tantost, si me hare mez chiens a ce mesel</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Qui par devant ma porte demaine tel cembel,</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>83</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Souvent se claime las, chetis, maleüreux</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>“Que feray, que diray, que pourray devenir?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Las, pourray je jamais de ce tourmant yssir?</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2865,7 +2961,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2940,7 +3036,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -3682,6 +3778,341 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>line_n</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>prev_line</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>line</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>next_line</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>85</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Puis a dit a son frere, sans point de demourer:</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>“Portez ce panyer en ung batel en la mer,</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Et puis si le laissiez tout a par luy aller.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>104</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>A l'abbé le porterent, si l'ont mis a raison:</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>“Sire, nous ne povons point de poisson peschier,</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Mais nous avons trouvé sur la mer ung panyer;</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>114</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>L'abbé regarde es tables, si dist ceste raison:</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>“Il est de noble lieu; il portera mon nom.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Se Dieu plaist il sera encore moult preudom.”</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>227</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>La chose lui conta, lequel fut en esmoy:</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>“Et non pourtant a lui je me combateray,</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Et se je le puis vaincre, foy que doy saint Martin,</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>258</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Puis est venu au conte, si lui dist a hault ton:</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>“Mon cheual avez mort, c'est trop grant traÿson.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Mais bien tost en arez le vostre guerredon.”</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>336</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Quant elle vit les tables, elle dit haultement:</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>“Mon filz m'a espousee! De dueil le cueur me fent.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Avecques moy sept ans a esté tellement.”</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>361</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Adonc recommenca la povre gent a braire.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>“Demourez avec nous, gentilz homs debonnaire.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Quant en voulez aller, forment nous doit desplaire.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>368</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Son aumosnier appelle, si lui dist doulcement:</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>“Donnez leur a chacun ung gros tournois d'argent.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Je m'en yray toudis, trop me font de tourment;</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>404</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Lors l'oste respondi, qui n'estoit point vilain:</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>“Pres de cy a vne ysle que vous verrez demain.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Il ya vne roche, je vous dy de certain,</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>424</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Puis a dit a son hoste moult debonairement:</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>“Or refermez la roche, tost et delivrement,</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Et men bailliez la clef, car je la vous demand.”</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>472</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Quant l'oste la regarde, si dist ceste raison:</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>“C'est la clef de la roche, sans variatïon,</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Ou j'enfermay Gregoire, qui tant estoit preudom.”</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>478</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Et il leur print a dire, sans gaires demourer:</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>“Sept ans a que il fut en la roche enfermé.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Je croy qu'il est piecha du siecle trespassé.”</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>492</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Et ilz lui respondirent a vne voix trestous:</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>“Vous en venrez, beau sire, maintenant avec nous,</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>En la cité de Romme; povoir arez sur tous.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>499</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Son hoste lui a dit, sans longue demourance:</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>“Beau sire veez la, n'en soyez en doubtance.”</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Quant il la vit si dist: “Dieu, qu'avez grant puissace!</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>548</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Devant lui est venue, haultement lui escrie:</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>“Pere, plus grant pecheresse ne fut onc mais ouÿe.”</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Saint Gregoire l'apelle, et lui dist: “Doulce amye,</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3815,7 +4246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -4010,7 +4441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -4083,99 +4514,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>line_n</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>prev_line</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>line</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>next_line</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
-        <v>151</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>L'annel boute en son dois, puis leur dist maintenant:</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>“Seigneurs, comment se porte l'eglise et la gent?”</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Et il ont respondu: “Sire, moult flebement.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>177</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>L'archevesque saint Leu si lui a repondu:</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>“Coulombe, belle suer, chascun si doit mater</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Sa charongne pour Dieu servir et hounourer.”</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>217</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Tout fu prest a cuilir, ce fu grace plainiere.</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>“Encore vous requier par sainte trinité</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Que toutes creatures qui seront tourmenté</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>